<commit_message>
Modified Files with values
</commit_message>
<xml_diff>
--- a/startups/startups.xlsx
+++ b/startups/startups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My-Github\Companies-Startups\startups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A900D8D-740B-4196-A465-C69D054506F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5DC4CC-AED2-4757-B760-F355487BEF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,13 +342,7 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>